<commit_message>
Battery SOC table added
</commit_message>
<xml_diff>
--- a/meta/word_count.xlsx
+++ b/meta/word_count.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsuch/Documents/GitHub/Embedded-AI/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B84A9B2-E1CA-6B4A-B74D-B828AC340C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B889B85-9DBF-9F42-A993-9DCCDAD6E299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="8520" windowWidth="27640" windowHeight="16940" xr2:uid="{0ADB3043-401F-AF49-B282-8B91DA08A523}"/>
+    <workbookView xWindow="16860" yWindow="8780" windowWidth="27640" windowHeight="16940" xr2:uid="{0ADB3043-401F-AF49-B282-8B91DA08A523}"/>
   </bookViews>
   <sheets>
     <sheet name="Word Count" sheetId="1" r:id="rId1"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,8 +779,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="6">
+        <v>45466</v>
+      </c>
+      <c r="B11" s="7">
+        <v>885</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
       <c r="G11" s="6"/>
@@ -1186,12 +1190,12 @@
       </c>
       <c r="B30" s="11">
         <f>SUM(B9:B29)+SUM(E9:E29)+SUM(H9:H29) + SUM(K9:K29) + SUM(N9:N29) + SUM(Q9:Q29)</f>
-        <v>1477</v>
+        <v>2362</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="13">
         <f>B30/80000</f>
-        <v>1.84625E-2</v>
+        <v>2.9524999999999999E-2</v>
       </c>
       <c r="S30" s="11" t="s">
         <v>6</v>
@@ -1232,7 +1236,7 @@
       </c>
       <c r="B32" s="16">
         <f>B30/(COUNT(B9:B28)+COUNT(E9:E28)+COUNT(H9:H28)+COUNT(K9:K28)+COUNT(N9:N28))</f>
-        <v>738.5</v>
+        <v>787.33333333333337</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>11</v>
@@ -1244,7 +1248,7 @@
       </c>
       <c r="B33" s="3">
         <f>88000-B30</f>
-        <v>86523</v>
+        <v>85638</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>13</v>
@@ -1254,7 +1258,7 @@
       </c>
       <c r="W33" s="14">
         <f>$T$30+$W$30-$B$30</f>
-        <v>-1477</v>
+        <v>-2362</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="19" x14ac:dyDescent="0.25">
@@ -1263,7 +1267,7 @@
       </c>
       <c r="B34" s="16">
         <f>B33/B32</f>
-        <v>117.16046039268788</v>
+        <v>108.76968670618119</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>16</v>
@@ -1275,7 +1279,7 @@
       </c>
       <c r="B35" s="18">
         <f ca="1">TODAY() + B34</f>
-        <v>45582.16046039269</v>
+        <v>45574.769686706182</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>18</v>
@@ -1287,7 +1291,7 @@
       </c>
       <c r="B37" s="16">
         <f>B33/12</f>
-        <v>7210.25</v>
+        <v>7136.5</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="19" x14ac:dyDescent="0.25">

</xml_diff>